<commit_message>
Updated Standard error bug
Former-commit-id: 400b4938292a12f3709f76aad65724e0a998b8f3
Former-commit-id: 32481c448a4e8d2d78ee732559f87fa80c21263a
</commit_message>
<xml_diff>
--- a/Plots_for_Paper_vmat/likelihoodcomparison.xlsx
+++ b/Plots_for_Paper_vmat/likelihoodcomparison.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -488,11 +488,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="-2093396920"/>
-        <c:axId val="-2093392792"/>
+        <c:axId val="2137780008"/>
+        <c:axId val="2137786792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2093396920"/>
+        <c:axId val="2137780008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -520,7 +520,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093392792"/>
+        <c:crossAx val="2137786792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -528,7 +528,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2093392792"/>
+        <c:axId val="2137786792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -557,7 +557,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093396920"/>
+        <c:crossAx val="2137780008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -793,11 +793,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-25"/>
-        <c:axId val="-2086238376"/>
-        <c:axId val="-2086046904"/>
+        <c:axId val="2137826312"/>
+        <c:axId val="2137829224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2086238376"/>
+        <c:axId val="2137826312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -806,7 +806,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2086046904"/>
+        <c:crossAx val="2137829224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -814,7 +814,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2086046904"/>
+        <c:axId val="2137829224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -824,7 +824,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2086238376"/>
+        <c:crossAx val="2137826312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -935,11 +935,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2093174312"/>
-        <c:axId val="-2110531960"/>
+        <c:axId val="2137809128"/>
+        <c:axId val="2137714168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2093174312"/>
+        <c:axId val="2137809128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -948,7 +948,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110531960"/>
+        <c:crossAx val="2137714168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -956,7 +956,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2110531960"/>
+        <c:axId val="2137714168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -967,7 +967,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2093174312"/>
+        <c:crossAx val="2137809128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1118,11 +1118,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="-2107799400"/>
-        <c:axId val="-2107741224"/>
+        <c:axId val="2137863464"/>
+        <c:axId val="2137868856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2107799400"/>
+        <c:axId val="2137863464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1149,7 +1149,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2107741224"/>
+        <c:crossAx val="2137868856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1157,7 +1157,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2107741224"/>
+        <c:axId val="2137868856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1185,7 +1185,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2107799400"/>
+        <c:crossAx val="2137863464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1657,7 +1657,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1799,7 +1799,7 @@
         <v>-1268191</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>-1268102</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>-1268065.99731736</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>-1267998.3999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1831,7 +1831,7 @@
         <v>-1267998.4840939001</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>-1268049.69</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>-1267997.5</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -1855,15 +1855,19 @@
         <v>-1274778</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>33</v>
       </c>
       <c r="B24">
         <v>-1264772.82</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24">
+        <f>B24-B25</f>
+        <v>18432.719999999972</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -1871,17 +1875,17 @@
         <v>-1283205.54</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:3">
       <c r="B26" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:3">
       <c r="B27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:3">
       <c r="B28" t="s">
         <v>29</v>
       </c>

</xml_diff>